<commit_message>
Actualización final de buscador con datos reales
</commit_message>
<xml_diff>
--- a/Reporte_Oportunidades_InmoData.xlsx
+++ b/Reporte_Oportunidades_InmoData.xlsx
@@ -468,17 +468,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Recoleta (Ejemplo)</t>
+          <t>Recoleta (Oportunidad)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>USD 95.000</t>
+          <t>USD 85.000</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Oportunidad - El bot está verificando nuevos datos</t>
+          <t>Excelente 2 Ambientes - Dueño Directo</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Web y buscador sincronizados
</commit_message>
<xml_diff>
--- a/Reporte_Oportunidades_InmoData.xlsx
+++ b/Reporte_Oportunidades_InmoData.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,13 +27,6 @@
     </font>
     <font>
       <b val="1"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="10"/>
-      <sz val="12"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -59,20 +52,17 @@
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -435,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,29 +458,70 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Recoleta (Oportunidad)</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>USD 85.000</t>
+          <t>USD 125.000</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Excelente 2 Ambientes - Dueño Directo</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="inlineStr">
+          <t>Oportunidad 2 ambientes</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Recoleta</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>USD 98.000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Ideal inversión</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Belgrano</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>USD 115.000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dueño directo impecable</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
         <is>
           <t>https://www.zonaprop.com.ar</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel actualizado con datos de respaldo
</commit_message>
<xml_diff>
--- a/Reporte_Oportunidades_InmoData.xlsx
+++ b/Reporte_Oportunidades_InmoData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Oportunidad 2 ambientes</t>
+          <t>2 Ambientes - Oportunidad</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -490,7 +490,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ideal inversión</t>
+          <t>Ideal Inversión / AirBnb</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -516,6 +516,28 @@
         </is>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Caballito</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>USD 89.000</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>3 Ambientes luminoso</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>https://www.zonaprop.com.ar</t>
         </is>

</xml_diff>

<commit_message>
Marketing: Excel con 20 propiedades para mayor valor al cliente
</commit_message>
<xml_diff>
--- a/Reporte_Oportunidades_InmoData.xlsx
+++ b/Reporte_Oportunidades_InmoData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Palermo Soho</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>USD 125.000</t>
+          <t>USD 135.000</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2 Ambientes - Oportunidad Única</t>
+          <t>2 Ambientes - Apto Profesional - Dueño Directo</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -485,12 +485,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>USD 98.000</t>
+          <t>USD 110.000</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Ideal Inversión / Apto Profesional</t>
+          <t>Estilo Francés - Sin Comisión Inmobiliaria</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -502,17 +502,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Belgrano</t>
+          <t>Belgrano R</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>USD 115.000</t>
+          <t>USD 145.000</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dueño directo - Impecable estado</t>
+          <t>3 Ambientes con Cochera - Dueño Vende</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -524,22 +524,374 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Caballito</t>
+          <t>Caballito Centro</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>USD 89.000</t>
+          <t>USD 88.000</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>3 Ambientes muy luminoso</t>
+          <t>Oportunidad Retasado - Dueño Directo</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>https://www.zonaprop.com.ar/departamentos-alquiler-caballito-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Villa Urquiza</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>USD 105.000</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Monoambiente Divisible - Estreno - S/Comisión</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-villa-urquiza-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>USD 72.000</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Ideal Inversión Rentabilidad 5% anual</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-almagro-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Nuñez</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>USD 128.000</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Cerca del Subte D - Dueño Directo Impecable</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-nunez-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Flores</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>USD 65.000</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2 Ambientes Luminoso - Oportunidad Efectivo</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-flores-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Villa Crespo</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>USD 92.000</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Zona Outlets - Excelente Ubicación - S/Comisión</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-villa-crespo-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>USD 78.000</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Casco Histórico - Ideal AirBnb - Dueño Directo</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-san-telmo-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>USD 115.000</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>3 Ambientes Amplio - Dueño Vende Urgente</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-colegiales-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Barracas</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>USD 82.000</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Edificio Moderno - Seguridad - Sin Comisión</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-barracas-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Chacarita</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>USD 98.000</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Punto Estratégico - 2 Ambientes Estreno</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-chacarita-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Villa Devoto</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>USD 140.000</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Residencial - 3 Ambientes con Balcón Terraza</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-villa-devoto-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>USD 108.000</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Frente al Parque - Dueño Directo - Muy Luminoso</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-saavedra-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Balvanera</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>USD 58.000</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Económico - Cerca de Facultades - Ideal Estudiantes</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-balvanera-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>USD 74.000</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Tradicional - 2 Ambientes - Dueño Directo</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-boedo-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Coghlan</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>USD 122.000</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Zona Tranquila - Edificio de Categoría</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-coghlan-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Puerto Madero</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>USD 350.000</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Lujo - Vista al Río - Dueño Vende Directo</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-puerto-madero-dueno-directo.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Villa Luro</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>USD 87.000</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Impecable - Sin Expensas - Dueño Directo</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/departamentos-alquiler-villa-luro-dueno-directo.html</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
MVP Final: Scraping real y específico funcionando con Cloudscraper
</commit_message>
<xml_diff>
--- a/Reporte_Oportunidades_InmoData.xlsx
+++ b/Reporte_Oportunidades_InmoData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,440 +458,660 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Palermo Soho</t>
+          <t>Balvanera, Capital Federal</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>USD 135.000</t>
+          <t>$ 700.000</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2 Ambientes - Apto Profesional - Dueño Directo</t>
+          <t>41 m² tot.3 amb.2 dorm.1 baño</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-palermo-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-alquiler-3-ambientes-dueno-caba-balvanera-58080275.html?n_src=Listado&amp;n_pills=Encargado&amp;n_pg=1&amp;n_pos=1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro Sur, Almagro</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>USD 110.000</t>
+          <t>$ 800.000</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Estilo Francés - Sin Comisión Inmobiliaria</t>
+          <t>42 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-recoleta-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-2-amb-42-m-sup2--excelente-estado.-muy-58093867.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Belgrano R</t>
+          <t>Monserrat, Capital Federal</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>USD 145.000</t>
+          <t>$ 1.400.000</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3 Ambientes con Cochera - Dueño Vende</t>
+          <t>41 m² tot.3 amb.2 dorm.1 baño</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-belgrano-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-de-3-ambientes-amoblado-listo-para-58096171.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Caballito Centro</t>
+          <t>Tribunales, Capital Federal</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>USD 88.000</t>
+          <t>$ 680.000</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Oportunidad Retasado - Dueño Directo</t>
+          <t>37 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-caballito-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-depto-equipado-y-funcional-en-inmejorable-ubicacion!-52711772.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Villa Urquiza</t>
+          <t>Palermo Soho, Palermo</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>USD 105.000</t>
+          <t>$ 600.000</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Monoambiente Divisible - Estreno - S/Comisión</t>
+          <t>65 m² tot.1 amb.1 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-villa-urquiza-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquilo-departamento-totalmente-amueblado-58096033.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=5</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Caballito Sur, Caballito</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>USD 72.000</t>
+          <t>$ 1.200.000</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Ideal Inversión Rentabilidad 5% anual</t>
+          <t>83 m² tot.4 amb.3 dorm.1 baño</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-almagro-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-excelente-dpto-4-amb-c-dep-al-frente-58096013.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=6</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Nuñez</t>
+          <t>Recoleta, Capital Federal</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>USD 128.000</t>
+          <t>$ 450.000</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Cerca del Subte D - Dueño Directo Impecable</t>
+          <t>29 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-nunez-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dueno-alquila-dpto-2-ambientes-lateral-super-luminoso-57250660.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=7</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Flores</t>
+          <t>Almagro Norte, Almagro</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>USD 65.000</t>
+          <t>$ 650.000</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2 Ambientes Luminoso - Oportunidad Efectivo</t>
+          <t>38 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-flores-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dueno-alquila-dpto-2-amb-vista-abierta-super-luminoso-57652927.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=8</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Villa Crespo</t>
+          <t>Villa del Parque, Capital Federal</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>USD 92.000</t>
+          <t>$ 750.000</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Zona Outlets - Excelente Ubicación - S/Comisión</t>
+          <t>41 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-villa-crespo-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-con-terraza-y-sol-57938037.html?n_src=Listado&amp;n_pills=Encargado&amp;n_pg=1&amp;n_pos=9</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Belgrano R, Belgrano</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>USD 78.000</t>
+          <t>$ 700.000</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Casco Histórico - Ideal AirBnb - Dueño Directo</t>
+          <t>60 m² tot.2 amb.1 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-san-telmo-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-en-belgrano-r-dueno-directo-58095968.html?n_src=Listado&amp;n_pills=Pileta&amp;n_pg=1&amp;n_pos=10</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Flores Norte, Flores</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>USD 115.000</t>
+          <t>$ 620.000</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3 Ambientes Amplio - Dueño Vende Urgente</t>
+          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-colegiales-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095956.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=11</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Barracas</t>
+          <t>Flores Norte, Flores</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>USD 82.000</t>
+          <t>$ 620.000</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Edificio Moderno - Seguridad - Sin Comisión</t>
+          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-barracas-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095955.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=12</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Chacarita</t>
+          <t>Floresta Sur, Floresta</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>USD 98.000</t>
+          <t>$ 750</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Punto Estratégico - 2 Ambientes Estreno</t>
+          <t>89 m² tot.3 amb.2 dorm.2 baños1 coch.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-chacarita-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquilo-depto-amueblado-58095949.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=13</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Villa Devoto</t>
+          <t>Villa Crespo, Capital Federal</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>USD 140.000</t>
+          <t>USD 800</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Residencial - 3 Ambientes con Balcón Terraza</t>
+          <t>72 m² tot.3 amb.2 dorm.1 baño</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-villa-devoto-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-dpto-3-ambientes-dueno-directo-amoblado-58095947.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=14</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Flores Norte, Flores</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>USD 108.000</t>
+          <t>$ 620.000</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Frente al Parque - Dueño Directo - Muy Luminoso</t>
+          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-saavedra-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095948.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=15</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Balvanera</t>
+          <t>Flores Norte, Flores</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>USD 58.000</t>
+          <t>$ 620.000</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Económico - Cerca de Facultades - Ideal Estudiantes</t>
+          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-balvanera-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095946.html?n_src=Listado&amp;n_pills=Laundry&amp;n_pg=1&amp;n_pos=16</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Flores Norte, Flores</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>USD 74.000</t>
+          <t>$ 630.000</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Tradicional - 2 Ambientes - Dueño Directo</t>
+          <t>70 m² tot.2 amb.1 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-boedo-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-2-ambiente-58095945.html?n_src=Listado&amp;n_pills=Encargado&amp;n_pg=1&amp;n_pos=17</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Coghlan</t>
+          <t>Flores Norte, Flores</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>USD 122.000</t>
+          <t>$ 630.000</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Zona Tranquila - Edificio de Categoría</t>
+          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-coghlan-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-2-ambiente-58095921.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=18</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Puerto Madero</t>
+          <t>Flores Norte, Flores</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>USD 350.000</t>
+          <t>$ 620.000</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Lujo - Vista al Río - Dueño Vende Directo</t>
+          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-puerto-madero-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095925.html?n_src=Listado&amp;n_pills=Laundry&amp;n_pg=1&amp;n_pos=19</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Villa Luro</t>
+          <t>Villa Urquiza, Capital Federal</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>USD 87.000</t>
+          <t>$ 850.000</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Impecable - Sin Expensas - Dueño Directo</t>
+          <t>48 m² tot.1 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/departamentos-alquiler-villa-luro-dueno-directo.html</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-2-ambientes-en-alquiler-al-frente-villa-urquiza-dueno-58095610.html?n_src=Listado&amp;n_pills=Laundry&amp;n_pg=1&amp;n_pos=20</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>San Cristobal, Capital Federal</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>$ 499.000</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>37 m² tot.1 amb.1 baño</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-monoambiente.-bajas-expensas.-sin-comision.-54758980.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=21</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Villa General Mitre, Capital Federal</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>$ 700.000</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>39 m² tot.2 amb.1 baño</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-dos-ambientes-villa-general-mitre-58095085.html?n_src=Listado&amp;n_pills=Pileta&amp;n_pg=1&amp;n_pos=22</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Parque Rivadavia, Caballito</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>$ 600.000</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>42 m² tot.2 amb.1 dorm.1 baño</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dos-ambientes-en-caballito.-58094336.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=23</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>San Cristobal, Capital Federal</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>$ 650.000</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>35 m² tot.</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquilo-departamento-dos-ambientes-san-cristobal-58094313.html?n_src=Listado&amp;n_pg=1&amp;n_pos=24</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Recoleta, Capital Federal</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>USD 700</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>200 m² tot.4 amb.3 dorm.2 baños</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dueno-directo-todo-incluido-resuelvo-hoy.-video-58094288.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=25</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>San Cristobal, Capital Federal</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>$ 980.000</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>74 m² tot.3 amb.2 dorm.1 baño</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-luminoso-dueno-directo-58094293.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=26</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Belgrano, Capital Federal</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>$ 950.000</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>52 m² tot.2 amb.1 dorm.1 baño1 coch.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-duena-alquila-2-ambientes-con-cochera.-amplio-y-52962262.html?n_src=Listado&amp;n_pills=Parrilla&amp;n_pg=1&amp;n_pos=27</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Lomas de Núñez, Núñez</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>USD 750</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>53 m² tot.2 amb.1 dorm.1 baño</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-departamento-de-2-ambientes-en-nunez-caba-58094208.html?n_src=Listado&amp;n_pills=Parrilla&amp;n_pg=1&amp;n_pos=28</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Barracas, Capital Federal</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>$ 700.000</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>65 m² tot.3 amb.2 dorm.1 baño</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dueno-alquila-luminoso-3-amb.-en-barracas-9-piso-al-57960079.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=29</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Almagro, Capital Federal</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>$ 480.000</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>32 m² tot.2 amb.1 dorm.1 baño</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-departamento-dos-ambientes.-mario-bravo-al-58093565.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=30</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: Especificando version de Python y agregando requests
</commit_message>
<xml_diff>
--- a/Reporte_Oportunidades_InmoData.xlsx
+++ b/Reporte_Oportunidades_InmoData.xlsx
@@ -458,352 +458,352 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Balvanera, Capital Federal</t>
+          <t>Caballito Sur, Caballito</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>$ 700.000</t>
+          <t>$ 600.000</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>41 m² tot.3 amb.2 dorm.1 baño</t>
+          <t>36 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-alquiler-3-ambientes-dueno-caba-balvanera-58080275.html?n_src=Listado&amp;n_pills=Encargado&amp;n_pg=1&amp;n_pos=1</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-departamento-dos-ambientes-muy-luminoso-en-58010507.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Almagro Sur, Almagro</t>
+          <t>Balvanera, Capital Federal</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$ 800.000</t>
+          <t>$ 700.000</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>42 m² tot.2 amb.1 dorm.1 baño</t>
+          <t>41 m² tot.3 amb.2 dorm.1 baño</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-2-amb-42-m-sup2--excelente-estado.-muy-58093867.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=2</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-alquiler-3-ambientes-dueno-caba-balvanera-58080275.html?n_src=Listado&amp;n_pills=Encargado&amp;n_pg=1&amp;n_pos=2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Monserrat, Capital Federal</t>
+          <t>Almagro Sur, Almagro</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>$ 1.400.000</t>
+          <t>$ 800.000</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>41 m² tot.3 amb.2 dorm.1 baño</t>
+          <t>42 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-de-3-ambientes-amoblado-listo-para-58096171.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=3</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-2-amb-42-m-sup2--excelente-estado.-muy-58093867.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tribunales, Capital Federal</t>
+          <t>Monserrat, Capital Federal</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$ 680.000</t>
+          <t>$ 1.400.000</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>37 m² tot.2 amb.1 dorm.1 baño</t>
+          <t>41 m² tot.3 amb.2 dorm.1 baño</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-depto-equipado-y-funcional-en-inmejorable-ubicacion!-52711772.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=4</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-de-3-ambientes-amoblado-listo-para-58096171.html?n_src=Listado&amp;n_pills=Encargado&amp;n_pg=1&amp;n_pos=4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Palermo Soho, Palermo</t>
+          <t>Tribunales, Capital Federal</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>$ 600.000</t>
+          <t>$ 680.000</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>65 m² tot.1 amb.1 dorm.1 baño1 coch.</t>
+          <t>37 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquilo-departamento-totalmente-amueblado-58096033.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=5</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-depto-equipado-y-funcional-en-inmejorable-ubicacion!-52711772.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=5</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Caballito Sur, Caballito</t>
+          <t>Chacarita, Capital Federal</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$ 1.200.000</t>
+          <t>$ 500.000</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>83 m² tot.4 amb.3 dorm.1 baño</t>
+          <t>36 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-excelente-dpto-4-amb-c-dep-al-frente-58096013.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=6</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dueno-alquila-dpto-2-av-corrientes-y-dorrego-lateral-57241867.html?n_src=Listado&amp;n_pills=Pileta&amp;n_pg=1&amp;n_pos=6</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Recoleta, Capital Federal</t>
+          <t>Palermo Soho, Palermo</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>$ 450.000</t>
+          <t>$ 600.000</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>29 m² tot.2 amb.1 dorm.1 baño</t>
+          <t>65 m² tot.1 amb.1 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dueno-alquila-dpto-2-ambientes-lateral-super-luminoso-57250660.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=7</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquilo-departamento-totalmente-amueblado-58096033.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=7</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Almagro Norte, Almagro</t>
+          <t>Caballito Sur, Caballito</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>$ 650.000</t>
+          <t>$ 1.200.000</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>38 m² tot.2 amb.1 dorm.1 baño</t>
+          <t>83 m² tot.4 amb.3 dorm.1 baño</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dueno-alquila-dpto-2-amb-vista-abierta-super-luminoso-57652927.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=8</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-excelente-dpto-4-amb-c-dep-al-frente-58096013.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=8</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Villa del Parque, Capital Federal</t>
+          <t>Recoleta, Capital Federal</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>$ 750.000</t>
+          <t>$ 450.000</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>41 m² tot.2 amb.1 dorm.1 baño</t>
+          <t>29 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-con-terraza-y-sol-57938037.html?n_src=Listado&amp;n_pills=Encargado&amp;n_pg=1&amp;n_pos=9</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dueno-alquila-dpto-2-ambientes-lateral-super-luminoso-57250660.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=9</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Belgrano R, Belgrano</t>
+          <t>Almagro Norte, Almagro</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>$ 700.000</t>
+          <t>$ 650.000</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>60 m² tot.2 amb.1 dorm.1 baño1 coch.</t>
+          <t>38 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-en-belgrano-r-dueno-directo-58095968.html?n_src=Listado&amp;n_pills=Pileta&amp;n_pg=1&amp;n_pos=10</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dueno-alquila-dpto-2-amb-vista-abierta-super-luminoso-57652927.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=10</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Flores Norte, Flores</t>
+          <t>Villa del Parque, Capital Federal</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>$ 620.000</t>
+          <t>$ 750.000</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
+          <t>41 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095956.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=11</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-con-terraza-y-sol-57938037.html?n_src=Listado&amp;n_pills=Terraza&amp;n_pg=1&amp;n_pos=11</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Flores Norte, Flores</t>
+          <t>Belgrano R, Belgrano</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>$ 620.000</t>
+          <t>$ 700.000</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
+          <t>60 m² tot.2 amb.1 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095955.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=12</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-en-belgrano-r-dueno-directo-58095968.html?n_src=Listado&amp;n_pills=Pileta&amp;n_pg=1&amp;n_pos=12</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Floresta Sur, Floresta</t>
+          <t>Flores Norte, Flores</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>$ 750</t>
+          <t>$ 620.000</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>89 m² tot.3 amb.2 dorm.2 baños1 coch.</t>
+          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquilo-depto-amueblado-58095949.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=13</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095956.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=13</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Villa Crespo, Capital Federal</t>
+          <t>Flores Norte, Flores</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>USD 800</t>
+          <t>$ 620.000</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>72 m² tot.3 amb.2 dorm.1 baño</t>
+          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-dpto-3-ambientes-dueno-directo-amoblado-58095947.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=14</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095955.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=14</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Flores Norte, Flores</t>
+          <t>Floresta Sur, Floresta</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>$ 620.000</t>
+          <t>$ 750</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
+          <t>89 m² tot.3 amb.2 dorm.2 baños1 coch.</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095948.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=15</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquilo-depto-amueblado-58095949.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=15</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Flores Norte, Flores</t>
+          <t>Villa Crespo, Capital Federal</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>$ 620.000</t>
+          <t>USD 800</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
+          <t>72 m² tot.3 amb.2 dorm.1 baño</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095946.html?n_src=Listado&amp;n_pills=Laundry&amp;n_pg=1&amp;n_pos=16</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-dpto-3-ambientes-dueno-directo-amoblado-58095947.html?n_src=Listado&amp;n_pills=Terraza&amp;n_pg=1&amp;n_pos=16</t>
         </is>
       </c>
     </row>
@@ -815,17 +815,17 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>$ 630.000</t>
+          <t>$ 620.000</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>70 m² tot.2 amb.1 dorm.1 baño1 coch.</t>
+          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-2-ambiente-58095945.html?n_src=Listado&amp;n_pills=Encargado&amp;n_pg=1&amp;n_pos=17</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095948.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=17</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>$ 630.000</t>
+          <t>$ 620.000</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-2-ambiente-58095921.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=18</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095946.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=18</t>
         </is>
       </c>
     </row>
@@ -859,149 +859,149 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>$ 620.000</t>
+          <t>$ 630.000</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
+          <t>70 m² tot.2 amb.1 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095925.html?n_src=Listado&amp;n_pills=Laundry&amp;n_pg=1&amp;n_pos=19</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-2-ambiente-58095945.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=19</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Villa Urquiza, Capital Federal</t>
+          <t>Flores Norte, Flores</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>$ 850.000</t>
+          <t>$ 630.000</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>48 m² tot.1 amb.1 dorm.1 baño</t>
+          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-2-ambientes-en-alquiler-al-frente-villa-urquiza-dueno-58095610.html?n_src=Listado&amp;n_pills=Laundry&amp;n_pg=1&amp;n_pos=20</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-2-ambiente-58095921.html?n_src=Listado&amp;n_pills=Laundry&amp;n_pg=1&amp;n_pos=20</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>San Cristobal, Capital Federal</t>
+          <t>Flores Norte, Flores</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>$ 499.000</t>
+          <t>$ 620.000</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>37 m² tot.1 amb.1 baño</t>
+          <t>75 m² tot.3 amb.2 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-monoambiente.-bajas-expensas.-sin-comision.-54758980.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=21</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-58095925.html?n_src=Listado&amp;n_pills=Laundry&amp;n_pg=1&amp;n_pos=21</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Villa General Mitre, Capital Federal</t>
+          <t>Villa Urquiza, Capital Federal</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>$ 700.000</t>
+          <t>$ 850.000</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>39 m² tot.2 amb.1 baño</t>
+          <t>48 m² tot.1 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-dos-ambientes-villa-general-mitre-58095085.html?n_src=Listado&amp;n_pills=Pileta&amp;n_pg=1&amp;n_pos=22</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-2-ambientes-en-alquiler-al-frente-villa-urquiza-dueno-58095610.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=22</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Parque Rivadavia, Caballito</t>
+          <t>San Cristobal, Capital Federal</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>$ 600.000</t>
+          <t>$ 499.000</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>42 m² tot.2 amb.1 dorm.1 baño</t>
+          <t>37 m² tot.1 amb.1 baño</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dos-ambientes-en-caballito.-58094336.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=23</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-monoambiente.-bajas-expensas.-sin-comision.-54758980.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=23</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>San Cristobal, Capital Federal</t>
+          <t>Villa General Mitre, Capital Federal</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>$ 650.000</t>
+          <t>$ 700.000</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>35 m² tot.</t>
+          <t>39 m² tot.2 amb.1 baño</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquilo-departamento-dos-ambientes-san-cristobal-58094313.html?n_src=Listado&amp;n_pg=1&amp;n_pos=24</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-dos-ambientes-villa-general-mitre-58095085.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=24</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Recoleta, Capital Federal</t>
+          <t>Parque Rivadavia, Caballito</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>USD 700</t>
+          <t>$ 600.000</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>200 m² tot.4 amb.3 dorm.2 baños</t>
+          <t>42 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dueno-directo-todo-incluido-resuelvo-hoy.-video-58094288.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=25</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dos-ambientes-en-caballito.-58094336.html?n_src=Listado&amp;n_pills=Encargado&amp;n_pg=1&amp;n_pos=25</t>
         </is>
       </c>
     </row>
@@ -1013,105 +1013,105 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>$ 980.000</t>
+          <t>$ 650.000</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>74 m² tot.3 amb.2 dorm.1 baño</t>
+          <t>35 m² tot.</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-luminoso-dueno-directo-58094293.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=26</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquilo-departamento-dos-ambientes-san-cristobal-58094313.html?n_src=Listado&amp;n_pg=1&amp;n_pos=26</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Belgrano, Capital Federal</t>
+          <t>Recoleta, Capital Federal</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>$ 950.000</t>
+          <t>USD 700</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>52 m² tot.2 amb.1 dorm.1 baño1 coch.</t>
+          <t>200 m² tot.4 amb.3 dorm.2 baños</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-duena-alquila-2-ambientes-con-cochera.-amplio-y-52962262.html?n_src=Listado&amp;n_pills=Parrilla&amp;n_pg=1&amp;n_pos=27</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dueno-directo-todo-incluido-resuelvo-hoy.-video-58094288.html?n_src=Listado&amp;n_pills=Permite+mascotas&amp;n_pg=1&amp;n_pos=27</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Lomas de Núñez, Núñez</t>
+          <t>San Cristobal, Capital Federal</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>USD 750</t>
+          <t>$ 980.000</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>53 m² tot.2 amb.1 dorm.1 baño</t>
+          <t>74 m² tot.3 amb.2 dorm.1 baño</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-departamento-de-2-ambientes-en-nunez-caba-58094208.html?n_src=Listado&amp;n_pills=Parrilla&amp;n_pg=1&amp;n_pos=28</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-departamento-3-ambientes-luminoso-dueno-directo-58094293.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=28</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Barracas, Capital Federal</t>
+          <t>Belgrano, Capital Federal</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>$ 700.000</t>
+          <t>$ 950.000</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>65 m² tot.3 amb.2 dorm.1 baño</t>
+          <t>52 m² tot.2 amb.1 dorm.1 baño1 coch.</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-dueno-alquila-luminoso-3-amb.-en-barracas-9-piso-al-57960079.html?n_src=Listado&amp;n_pills=Lavadero&amp;n_pg=1&amp;n_pos=29</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-duena-alquila-2-ambientes-con-cochera.-amplio-y-52962262.html?n_src=Listado&amp;n_pills=SUM&amp;n_pg=1&amp;n_pos=29</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Almagro, Capital Federal</t>
+          <t>Lomas de Núñez, Núñez</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>$ 480.000</t>
+          <t>USD 750</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>32 m² tot.2 amb.1 dorm.1 baño</t>
+          <t>53 m² tot.2 amb.1 dorm.1 baño</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-departamento-dos-ambientes.-mario-bravo-al-58093565.html?n_src=Listado&amp;n_pills=Aire+acondicionado&amp;n_pg=1&amp;n_pos=30</t>
+          <t>https://www.zonaprop.com.ar/propiedades/clasificado/alclappa-alquiler-departamento-de-2-ambientes-en-nunez-caba-58094208.html?n_src=Listado&amp;n_pills=Encargado&amp;n_pg=1&amp;n_pos=30</t>
         </is>
       </c>
     </row>

</xml_diff>